<commit_message>
Remove stray shaded cell.
</commit_message>
<xml_diff>
--- a/Pathfinder-Analyser.xlsx
+++ b/Pathfinder-Analyser.xlsx
@@ -354,7 +354,9 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -369,7 +371,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -475,7 +477,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Barebranch" xfId="20"/>
     <cellStyle name="Transitional" xfId="21"/>
-    <cellStyle name="ConditionalStyle_3" xfId="22"/>
+    <cellStyle name="ConditionalStyle_3 1" xfId="22"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -734,7 +736,7 @@
   <dimension ref="A1:AK33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fix bug in summer/winter column headings.
</commit_message>
<xml_diff>
--- a/Pathfinder-Analyser.xlsx
+++ b/Pathfinder-Analyser.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="58">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t xml:space="preserve">Site %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summer</t>
   </si>
   <si>
     <t xml:space="preserve">Bare</t>
@@ -371,7 +377,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,7 +409,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -625,7 +631,7 @@
   </sheetPr>
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -735,8 +741,8 @@
   </sheetPr>
   <dimension ref="A1:AK33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -862,25 +868,23 @@
       <c r="AD5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AE5" s="11" t="str">
-        <f aca="false">IF(F3&lt;0, "Summer", "Winter")</f>
-        <v>Winter</v>
-      </c>
-      <c r="AF5" s="11" t="str">
-        <f aca="false">IF(F3&lt;0,"Winter","Summer")</f>
-        <v>Summer</v>
+      <c r="AE5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF5" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AI5" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AJ5" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AK5" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,10 +977,10 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AK6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,10 +1065,10 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AK7" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1153,10 +1157,10 @@
         <v>1</v>
       </c>
       <c r="AJ8" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AK8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,10 +1249,10 @@
         <v>0</v>
       </c>
       <c r="AJ9" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AK9" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,10 +1524,10 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AK12" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,10 +1620,10 @@
         <v>1</v>
       </c>
       <c r="AJ13" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AK13" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1988,7 +1992,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
@@ -2076,13 +2080,11 @@
       <c r="AD21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AE21" s="11" t="str">
-        <f aca="false">IF(F19&lt;0, "Summer", "Winter")</f>
-        <v>Summer</v>
-      </c>
-      <c r="AF21" s="11" t="str">
-        <f aca="false">IF(F19&lt;0,"Winter","Summer")</f>
-        <v>Winter</v>
+      <c r="AE21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF21" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3223,7 +3225,7 @@
   </sheetPr>
   <dimension ref="F9:F17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3257,7 +3259,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3283,7 +3285,7 @@
   </sheetPr>
   <dimension ref="A1:AD44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3298,7 +3300,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,7 +3367,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3438,7 +3440,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -3511,7 +3513,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3584,7 +3586,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3661,7 +3663,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3738,7 +3740,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3819,7 +3821,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3900,7 +3902,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3981,7 +3983,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="n">
@@ -4066,7 +4068,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="n">
@@ -4151,7 +4153,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="n">
@@ -4236,7 +4238,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>1</v>
@@ -4325,7 +4327,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4392,7 +4394,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4465,7 +4467,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -4538,7 +4540,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -4615,7 +4617,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4692,7 +4694,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4769,7 +4771,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -4850,7 +4852,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -4931,7 +4933,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -5012,7 +5014,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -5093,7 +5095,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -5174,7 +5176,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -5255,7 +5257,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="n">
@@ -5340,7 +5342,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5407,7 +5409,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -5480,7 +5482,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -5557,7 +5559,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -5634,7 +5636,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -5715,7 +5717,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -5796,7 +5798,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -5877,7 +5879,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -5958,7 +5960,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -6039,7 +6041,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -6120,7 +6122,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="n">
@@ -6205,7 +6207,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="n">
@@ -6290,7 +6292,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B44" s="2" t="n">
         <v>1</v>
@@ -6437,7 +6439,7 @@
   </sheetPr>
   <dimension ref="A1:AE174"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -6454,15 +6456,15 @@
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N1" s="25"/>
       <c r="O1" s="26"/>
       <c r="AD1" s="24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AE1" s="24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6527,7 +6529,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -6608,7 +6610,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -6689,7 +6691,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -6770,7 +6772,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -6851,7 +6853,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -6932,7 +6934,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -7013,7 +7015,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -7094,7 +7096,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -7175,7 +7177,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -7256,7 +7258,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -7337,7 +7339,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -7418,7 +7420,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -7499,7 +7501,7 @@
     </row>
     <row r="16" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N16" s="25"/>
       <c r="O16" s="26"/>
@@ -7566,7 +7568,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -7647,7 +7649,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -7728,7 +7730,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -7809,7 +7811,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -7890,7 +7892,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -7971,7 +7973,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -8052,7 +8054,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -8133,7 +8135,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -8214,7 +8216,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -8295,7 +8297,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -8376,7 +8378,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -8457,7 +8459,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -8538,7 +8540,7 @@
     </row>
     <row r="31" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N31" s="25"/>
       <c r="O31" s="26"/>
@@ -8605,7 +8607,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -8686,7 +8688,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -8767,7 +8769,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -8848,7 +8850,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -8929,7 +8931,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -9010,7 +9012,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -9091,7 +9093,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -9172,7 +9174,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -9253,7 +9255,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -9334,7 +9336,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -9413,12 +9415,12 @@
         <v>X</v>
       </c>
       <c r="AE42" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -9497,12 +9499,12 @@
         <v>X</v>
       </c>
       <c r="AE43" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -9581,12 +9583,12 @@
         <v>X</v>
       </c>
       <c r="AE44" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N46" s="25"/>
       <c r="O46" s="26"/>
@@ -9653,7 +9655,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -9730,7 +9732,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -9811,7 +9813,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -9892,7 +9894,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -9973,7 +9975,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -10054,7 +10056,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -10135,7 +10137,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -10216,7 +10218,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -10297,7 +10299,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -10378,7 +10380,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -10459,7 +10461,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -10540,7 +10542,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -10621,7 +10623,7 @@
     </row>
     <row r="61" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N61" s="25"/>
       <c r="O61" s="26"/>
@@ -10688,7 +10690,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -10765,7 +10767,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -10842,7 +10844,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -10919,7 +10921,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -10994,7 +10996,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -11075,7 +11077,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -11156,7 +11158,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -11237,7 +11239,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -11318,7 +11320,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -11399,7 +11401,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -11480,7 +11482,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="n">
@@ -11565,7 +11567,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="n">
@@ -11650,7 +11652,7 @@
     </row>
     <row r="76" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="N76" s="25"/>
       <c r="O76" s="26"/>
@@ -11717,7 +11719,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -11790,7 +11792,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -11863,7 +11865,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -11934,7 +11936,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -12009,7 +12011,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -12086,7 +12088,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -12167,7 +12169,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -12248,7 +12250,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -12329,7 +12331,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="n">
@@ -12414,7 +12416,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="n">
@@ -12499,7 +12501,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2" t="n">
@@ -12584,7 +12586,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2" t="n">
@@ -12669,7 +12671,7 @@
     </row>
     <row r="91" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N91" s="25"/>
       <c r="O91" s="26"/>
@@ -12736,7 +12738,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -12809,7 +12811,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -12886,7 +12888,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -12963,7 +12965,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -13038,7 +13040,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -13119,7 +13121,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -13200,7 +13202,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -13281,7 +13283,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -13362,7 +13364,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -13443,7 +13445,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="n">
@@ -13528,7 +13530,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2" t="n">
@@ -13613,7 +13615,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="n">
@@ -13698,7 +13700,7 @@
     </row>
     <row r="106" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N106" s="25"/>
       <c r="O106" s="26"/>
@@ -13765,7 +13767,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -13837,7 +13839,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -13914,7 +13916,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -13991,7 +13993,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -14072,7 +14074,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -14153,7 +14155,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -14234,7 +14236,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -14315,7 +14317,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -14396,7 +14398,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -14477,7 +14479,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="2" t="n">
@@ -14562,7 +14564,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="2" t="n">
@@ -14647,7 +14649,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B119" s="2" t="n">
         <v>1</v>
@@ -14736,7 +14738,7 @@
     </row>
     <row r="121" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N121" s="25"/>
       <c r="O121" s="26"/>
@@ -14803,7 +14805,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -14875,7 +14877,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -14948,7 +14950,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -15025,7 +15027,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -15102,7 +15104,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -15179,7 +15181,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -15260,7 +15262,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -15341,7 +15343,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -15422,7 +15424,7 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -15503,7 +15505,7 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -15584,7 +15586,7 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -15665,7 +15667,7 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="2" t="n">
@@ -15750,7 +15752,7 @@
     </row>
     <row r="136" s="24" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N136" s="25"/>
       <c r="O136" s="26"/>
@@ -15817,7 +15819,7 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -15889,7 +15891,7 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -15962,7 +15964,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -16035,7 +16037,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -16112,7 +16114,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -16189,7 +16191,7 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -16270,7 +16272,7 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -16351,7 +16353,7 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -16432,7 +16434,7 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" s="2" t="n">
@@ -16517,7 +16519,7 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" s="2" t="n">
@@ -16602,7 +16604,7 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" s="2" t="n">
@@ -16687,7 +16689,7 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B149" s="2" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Update instructions on the Instructions worksheet.
</commit_message>
<xml_diff>
--- a/Pathfinder-Analyser.xlsx
+++ b/Pathfinder-Analyser.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">Instructions</t>
   </si>
   <si>
-    <t xml:space="preserve">Make sure to enter the site latitude on the working sheet (negative for southern hemisphere, positive for northern)</t>
+    <t xml:space="preserve">Make sure to enter the site hemisphere on the working sheet</t>
   </si>
   <si>
     <t xml:space="preserve">For solid objects and evergreens:</t>
@@ -435,7 +435,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -463,7 +463,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -601,7 +601,7 @@
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <color rgb="00FFFFFF"/>
+        <color rgb="FFFFFFFF"/>
         <sz val="10"/>
         <u val="none"/>
       </font>
@@ -610,7 +610,6 @@
           <bgColor rgb="FFE5E5E5"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
@@ -694,8 +693,8 @@
   </sheetPr>
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -804,7 +803,7 @@
   </sheetPr>
   <dimension ref="A1:AL33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Shade summer/winter reduction factor cells in blue.
</commit_message>
<xml_diff>
--- a/Pathfinder-Analyser.xlsx
+++ b/Pathfinder-Analyser.xlsx
@@ -382,7 +382,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -456,6 +456,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -686,7 +690,7 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="2" sqref="AE6:AF6 AE22:AF22 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -796,7 +800,7 @@
   <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="N16" activeCellId="2" sqref="AE6:AF6 AE22:AF22 N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1015,11 +1019,11 @@
         <f aca="false">SUM(B6:AC6)</f>
         <v>83</v>
       </c>
-      <c r="AE6" s="18" t="n">
+      <c r="AE6" s="19" t="n">
         <f aca="false">AVERAGE(AD8,AD6,AD7,AD9,AD11,AD13)</f>
         <v>85.25</v>
       </c>
-      <c r="AF6" s="18" t="n">
+      <c r="AF6" s="19" t="n">
         <f aca="false">AVERAGE(AD15,AD17,AD16,AD14,AD12,AD10)</f>
         <v>92.3333333333333</v>
       </c>
@@ -1926,7 +1930,7 @@
       <c r="R16" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="S16" s="19" t="n">
+      <c r="S16" s="20" t="n">
         <v>6</v>
       </c>
       <c r="T16" s="15" t="n">
@@ -2076,7 +2080,7 @@
       <c r="E19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="20"/>
+      <c r="F19" s="21"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2164,7 +2168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="str">
         <f aca="false">IF(D19="S", "JUN", "DEC")</f>
         <v>JUN</v>
@@ -2237,11 +2241,11 @@
         <f aca="false">SUM(B22:AC22)</f>
         <v>74.5</v>
       </c>
-      <c r="AE22" s="18" t="n">
+      <c r="AE22" s="19" t="n">
         <f aca="false">AVERAGE(AD24,AD22,AD23,AD25,AD27,AD29)</f>
         <v>83.8333333333333</v>
       </c>
-      <c r="AF22" s="18" t="n">
+      <c r="AF22" s="19" t="n">
         <f aca="false">AVERAGE(AD31,AD33,AD32,AD30,AD28,AD26)</f>
         <v>93.9166666666667</v>
       </c>
@@ -3287,7 +3291,7 @@
       <formula>$AI22=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:AC33 B6:AC15 B17:AC17 B16:R16 T16:AC16">
+  <conditionalFormatting sqref="B22:AC33 G6:AC15 G17:AC17 G16:R16 T16:AC16 B6:F17">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND(NOT(ISBLANK(B6)), B6=0)</formula>
     </cfRule>
@@ -3328,7 +3332,7 @@
   <dimension ref="F9:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="2" sqref="AE6:AF6 AE22:AF22 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3337,10 +3341,10 @@
   </cols>
   <sheetData>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="21"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="21"/>
+      <c r="F10" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -3362,7 +3366,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="AE6:AF6 AE22:AF22 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3388,14 +3392,14 @@
   <dimension ref="A1:AD44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="2" sqref="AE6:AF6 AE22:AF22 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="22" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="23" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="23" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="24" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="16" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="0" width="10.59"/>
   </cols>
@@ -3499,10 +3503,10 @@
       <c r="M3" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="N3" s="24" t="n">
+      <c r="N3" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="O3" s="25" t="n">
+      <c r="O3" s="26" t="n">
         <v>9</v>
       </c>
       <c r="P3" s="2" t="n">
@@ -3572,10 +3576,10 @@
       <c r="M4" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N4" s="24" t="n">
+      <c r="N4" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="O4" s="25" t="n">
+      <c r="O4" s="26" t="n">
         <v>9</v>
       </c>
       <c r="P4" s="2" t="n">
@@ -3645,10 +3649,10 @@
       <c r="M5" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N5" s="24" t="n">
+      <c r="N5" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="O5" s="25" t="n">
+      <c r="O5" s="26" t="n">
         <v>9</v>
       </c>
       <c r="P5" s="2" t="n">
@@ -3720,10 +3724,10 @@
       <c r="M6" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N6" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O6" s="25" t="n">
+      <c r="N6" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O6" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P6" s="2" t="n">
@@ -3797,10 +3801,10 @@
       <c r="M7" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N7" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O7" s="25" t="n">
+      <c r="N7" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O7" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P7" s="2" t="n">
@@ -3876,10 +3880,10 @@
       <c r="M8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N8" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O8" s="25" t="n">
+      <c r="N8" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O8" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P8" s="2" t="n">
@@ -3957,10 +3961,10 @@
       <c r="M9" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N9" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O9" s="25" t="n">
+      <c r="N9" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O9" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P9" s="2" t="n">
@@ -4038,10 +4042,10 @@
       <c r="M10" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N10" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O10" s="25" t="n">
+      <c r="N10" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O10" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P10" s="2" t="n">
@@ -4121,10 +4125,10 @@
       <c r="M11" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N11" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O11" s="25" t="n">
+      <c r="N11" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O11" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P11" s="2" t="n">
@@ -4206,10 +4210,10 @@
       <c r="M12" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N12" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O12" s="25" t="n">
+      <c r="N12" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O12" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P12" s="2" t="n">
@@ -4291,10 +4295,10 @@
       <c r="M13" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N13" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O13" s="25" t="n">
+      <c r="N13" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O13" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P13" s="2" t="n">
@@ -4378,10 +4382,10 @@
       <c r="M14" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N14" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O14" s="25" t="n">
+      <c r="N14" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O14" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P14" s="2" t="n">
@@ -4526,10 +4530,10 @@
       <c r="M18" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N18" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O18" s="25" t="n">
+      <c r="N18" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O18" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P18" s="2" t="n">
@@ -4599,10 +4603,10 @@
       <c r="M19" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N19" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O19" s="25" t="n">
+      <c r="N19" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O19" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P19" s="2" t="n">
@@ -4674,10 +4678,10 @@
       <c r="M20" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N20" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O20" s="25" t="n">
+      <c r="N20" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O20" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P20" s="2" t="n">
@@ -4751,10 +4755,10 @@
       <c r="M21" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N21" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O21" s="25" t="n">
+      <c r="N21" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O21" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P21" s="2" t="n">
@@ -4828,10 +4832,10 @@
       <c r="M22" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N22" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O22" s="25" t="n">
+      <c r="N22" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O22" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P22" s="2" t="n">
@@ -4907,10 +4911,10 @@
       <c r="M23" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N23" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O23" s="25" t="n">
+      <c r="N23" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O23" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P23" s="2" t="n">
@@ -4988,10 +4992,10 @@
       <c r="M24" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N24" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O24" s="25" t="n">
+      <c r="N24" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O24" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P24" s="2" t="n">
@@ -5069,10 +5073,10 @@
       <c r="M25" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N25" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O25" s="25" t="n">
+      <c r="N25" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O25" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P25" s="2" t="n">
@@ -5150,10 +5154,10 @@
       <c r="M26" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N26" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O26" s="25" t="n">
+      <c r="N26" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O26" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P26" s="2" t="n">
@@ -5231,10 +5235,10 @@
       <c r="M27" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N27" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O27" s="25" t="n">
+      <c r="N27" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O27" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P27" s="2" t="n">
@@ -5312,10 +5316,10 @@
       <c r="M28" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N28" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O28" s="25" t="n">
+      <c r="N28" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O28" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P28" s="2" t="n">
@@ -5395,10 +5399,10 @@
       <c r="M29" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N29" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O29" s="25" t="n">
+      <c r="N29" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O29" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P29" s="2" t="n">
@@ -5541,10 +5545,10 @@
       <c r="M33" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N33" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O33" s="25" t="n">
+      <c r="N33" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O33" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P33" s="2" t="n">
@@ -5616,10 +5620,10 @@
       <c r="M34" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N34" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O34" s="25" t="n">
+      <c r="N34" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O34" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P34" s="2" t="n">
@@ -5693,10 +5697,10 @@
       <c r="M35" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N35" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O35" s="25" t="n">
+      <c r="N35" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O35" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P35" s="2" t="n">
@@ -5772,10 +5776,10 @@
       <c r="M36" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N36" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O36" s="25" t="n">
+      <c r="N36" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O36" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P36" s="2" t="n">
@@ -5853,10 +5857,10 @@
       <c r="M37" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N37" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O37" s="25" t="n">
+      <c r="N37" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O37" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P37" s="2" t="n">
@@ -5934,10 +5938,10 @@
       <c r="M38" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N38" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O38" s="25" t="n">
+      <c r="N38" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O38" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P38" s="2" t="n">
@@ -6015,10 +6019,10 @@
       <c r="M39" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N39" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O39" s="25" t="n">
+      <c r="N39" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O39" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P39" s="2" t="n">
@@ -6096,10 +6100,10 @@
       <c r="M40" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N40" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O40" s="25" t="n">
+      <c r="N40" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O40" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P40" s="2" t="n">
@@ -6177,10 +6181,10 @@
       <c r="M41" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N41" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O41" s="25" t="n">
+      <c r="N41" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O41" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P41" s="2" t="n">
@@ -6260,10 +6264,10 @@
       <c r="M42" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N42" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O42" s="25" t="n">
+      <c r="N42" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O42" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P42" s="2" t="n">
@@ -6345,10 +6349,10 @@
       <c r="M43" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N43" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O43" s="25" t="n">
+      <c r="N43" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O43" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P43" s="2" t="n">
@@ -6432,10 +6436,10 @@
       <c r="M44" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N44" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O44" s="25" t="n">
+      <c r="N44" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O44" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P44" s="2" t="n">
@@ -6542,30 +6546,30 @@
   <dimension ref="A1:AE174"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="2" sqref="AE6:AF6 AE22:AF22 G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="22" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="23" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="23" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="24" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="16" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="6.84"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="31" style="0" width="10.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="32" style="0" width="10.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+    <row r="1" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="28"/>
-      <c r="AD1" s="26" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="29"/>
+      <c r="AD1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="26" t="s">
+      <c r="AE1" s="27" t="s">
         <v>50</v>
       </c>
     </row>
@@ -6665,10 +6669,10 @@
       <c r="M3" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N3" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O3" s="25" t="n">
+      <c r="N3" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O3" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P3" s="2" t="n">
@@ -6746,10 +6750,10 @@
       <c r="M4" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N4" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O4" s="25" t="n">
+      <c r="N4" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O4" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P4" s="2" t="n">
@@ -6827,10 +6831,10 @@
       <c r="M5" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N5" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O5" s="25" t="n">
+      <c r="N5" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O5" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P5" s="2" t="n">
@@ -6908,10 +6912,10 @@
       <c r="M6" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N6" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O6" s="25" t="n">
+      <c r="N6" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O6" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P6" s="2" t="n">
@@ -6989,10 +6993,10 @@
       <c r="M7" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N7" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O7" s="25" t="n">
+      <c r="N7" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O7" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P7" s="2" t="n">
@@ -7070,10 +7074,10 @@
       <c r="M8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N8" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O8" s="25" t="n">
+      <c r="N8" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O8" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P8" s="2" t="n">
@@ -7151,10 +7155,10 @@
       <c r="M9" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N9" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O9" s="25" t="n">
+      <c r="N9" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O9" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P9" s="2" t="n">
@@ -7232,10 +7236,10 @@
       <c r="M10" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N10" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O10" s="25" t="n">
+      <c r="N10" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O10" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P10" s="2" t="n">
@@ -7313,10 +7317,10 @@
       <c r="M11" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N11" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O11" s="25" t="n">
+      <c r="N11" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O11" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P11" s="2" t="n">
@@ -7394,10 +7398,10 @@
       <c r="M12" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N12" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O12" s="25" t="n">
+      <c r="N12" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O12" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P12" s="2" t="n">
@@ -7475,10 +7479,10 @@
       <c r="M13" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N13" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O13" s="25" t="n">
+      <c r="N13" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O13" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P13" s="2" t="n">
@@ -7556,10 +7560,10 @@
       <c r="M14" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N14" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O14" s="25" t="n">
+      <c r="N14" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O14" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P14" s="2" t="n">
@@ -7601,12 +7605,12 @@
         <v/>
       </c>
     </row>
-    <row r="16" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26" t="s">
+    <row r="16" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="N16" s="27"/>
-      <c r="O16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
@@ -7704,10 +7708,10 @@
       <c r="M18" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N18" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O18" s="25" t="n">
+      <c r="N18" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O18" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P18" s="2" t="n">
@@ -7785,10 +7789,10 @@
       <c r="M19" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N19" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O19" s="25" t="n">
+      <c r="N19" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O19" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P19" s="2" t="n">
@@ -7866,10 +7870,10 @@
       <c r="M20" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N20" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O20" s="25" t="n">
+      <c r="N20" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O20" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P20" s="2" t="n">
@@ -7947,10 +7951,10 @@
       <c r="M21" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N21" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O21" s="25" t="n">
+      <c r="N21" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O21" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P21" s="2" t="n">
@@ -8028,10 +8032,10 @@
       <c r="M22" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N22" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O22" s="25" t="n">
+      <c r="N22" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O22" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P22" s="2" t="n">
@@ -8109,10 +8113,10 @@
       <c r="M23" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N23" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O23" s="25" t="n">
+      <c r="N23" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O23" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P23" s="2" t="n">
@@ -8190,10 +8194,10 @@
       <c r="M24" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N24" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O24" s="25" t="n">
+      <c r="N24" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O24" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P24" s="2" t="n">
@@ -8271,10 +8275,10 @@
       <c r="M25" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N25" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O25" s="25" t="n">
+      <c r="N25" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O25" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P25" s="2" t="n">
@@ -8352,10 +8356,10 @@
       <c r="M26" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N26" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O26" s="25" t="n">
+      <c r="N26" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O26" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P26" s="2" t="n">
@@ -8433,10 +8437,10 @@
       <c r="M27" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N27" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O27" s="25" t="n">
+      <c r="N27" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O27" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P27" s="2" t="n">
@@ -8514,10 +8518,10 @@
       <c r="M28" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N28" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O28" s="25" t="n">
+      <c r="N28" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O28" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P28" s="2" t="n">
@@ -8595,10 +8599,10 @@
       <c r="M29" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N29" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O29" s="25" t="n">
+      <c r="N29" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O29" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P29" s="2" t="n">
@@ -8640,12 +8644,12 @@
         <v/>
       </c>
     </row>
-    <row r="31" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26" t="s">
+    <row r="31" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="N31" s="27"/>
-      <c r="O31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
@@ -8743,10 +8747,10 @@
       <c r="M33" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N33" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O33" s="25" t="n">
+      <c r="N33" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O33" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P33" s="2" t="n">
@@ -8824,10 +8828,10 @@
       <c r="M34" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N34" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O34" s="25" t="n">
+      <c r="N34" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O34" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P34" s="2" t="n">
@@ -8905,10 +8909,10 @@
       <c r="M35" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N35" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O35" s="25" t="n">
+      <c r="N35" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O35" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P35" s="2" t="n">
@@ -8986,10 +8990,10 @@
       <c r="M36" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N36" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O36" s="25" t="n">
+      <c r="N36" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O36" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P36" s="2" t="n">
@@ -9067,10 +9071,10 @@
       <c r="M37" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N37" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O37" s="25" t="n">
+      <c r="N37" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O37" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P37" s="2" t="n">
@@ -9148,10 +9152,10 @@
       <c r="M38" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N38" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O38" s="25" t="n">
+      <c r="N38" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O38" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P38" s="2" t="n">
@@ -9229,10 +9233,10 @@
       <c r="M39" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N39" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O39" s="25" t="n">
+      <c r="N39" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O39" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P39" s="2" t="n">
@@ -9310,10 +9314,10 @@
       <c r="M40" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N40" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O40" s="25" t="n">
+      <c r="N40" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O40" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P40" s="2" t="n">
@@ -9391,10 +9395,10 @@
       <c r="M41" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N41" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O41" s="25" t="n">
+      <c r="N41" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O41" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P41" s="2" t="n">
@@ -9472,10 +9476,10 @@
       <c r="M42" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N42" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O42" s="25" t="n">
+      <c r="N42" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O42" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P42" s="2" t="n">
@@ -9556,10 +9560,10 @@
       <c r="M43" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N43" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O43" s="25" t="n">
+      <c r="N43" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O43" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P43" s="2" t="n">
@@ -9640,10 +9644,10 @@
       <c r="M44" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N44" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O44" s="25" t="n">
+      <c r="N44" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O44" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P44" s="2" t="n">
@@ -9688,12 +9692,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="26" t="s">
+    <row r="46" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N46" s="27"/>
-      <c r="O46" s="28"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="29"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
@@ -9789,10 +9793,10 @@
       <c r="M48" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N48" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O48" s="25" t="n">
+      <c r="N48" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O48" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P48" s="2" t="n">
@@ -9868,10 +9872,10 @@
       <c r="M49" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N49" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O49" s="25" t="n">
+      <c r="N49" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O49" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P49" s="2" t="n">
@@ -9949,10 +9953,10 @@
       <c r="M50" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N50" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O50" s="25" t="n">
+      <c r="N50" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O50" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P50" s="2" t="n">
@@ -10030,10 +10034,10 @@
       <c r="M51" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N51" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O51" s="25" t="n">
+      <c r="N51" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O51" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P51" s="2" t="n">
@@ -10111,10 +10115,10 @@
       <c r="M52" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N52" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O52" s="25" t="n">
+      <c r="N52" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O52" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P52" s="2" t="n">
@@ -10192,10 +10196,10 @@
       <c r="M53" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N53" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O53" s="25" t="n">
+      <c r="N53" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O53" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P53" s="2" t="n">
@@ -10273,10 +10277,10 @@
       <c r="M54" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N54" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O54" s="25" t="n">
+      <c r="N54" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O54" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P54" s="2" t="n">
@@ -10354,10 +10358,10 @@
       <c r="M55" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N55" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O55" s="25" t="n">
+      <c r="N55" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O55" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P55" s="2" t="n">
@@ -10435,10 +10439,10 @@
       <c r="M56" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N56" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O56" s="25" t="n">
+      <c r="N56" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O56" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P56" s="2" t="n">
@@ -10516,10 +10520,10 @@
       <c r="M57" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N57" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O57" s="25" t="n">
+      <c r="N57" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O57" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P57" s="2" t="n">
@@ -10597,10 +10601,10 @@
       <c r="M58" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N58" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O58" s="25" t="n">
+      <c r="N58" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O58" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P58" s="2" t="n">
@@ -10678,10 +10682,10 @@
       <c r="M59" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N59" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O59" s="25" t="n">
+      <c r="N59" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O59" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P59" s="2" t="n">
@@ -10723,12 +10727,12 @@
         <v/>
       </c>
     </row>
-    <row r="61" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="26" t="s">
+    <row r="61" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="N61" s="27"/>
-      <c r="O61" s="28"/>
+      <c r="N61" s="28"/>
+      <c r="O61" s="29"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
@@ -10824,10 +10828,10 @@
       <c r="M63" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N63" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O63" s="25" t="n">
+      <c r="N63" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O63" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P63" s="2" t="n">
@@ -10901,10 +10905,10 @@
       <c r="M64" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N64" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O64" s="25" t="n">
+      <c r="N64" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O64" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P64" s="2" t="n">
@@ -10978,10 +10982,10 @@
       <c r="M65" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N65" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O65" s="25" t="n">
+      <c r="N65" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O65" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P65" s="2" t="n">
@@ -11054,10 +11058,10 @@
       <c r="M66" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N66" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O66" s="25" t="n">
+      <c r="N66" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O66" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P66" s="2" t="n">
@@ -11132,10 +11136,10 @@
       <c r="M67" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N67" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O67" s="25" t="n">
+      <c r="N67" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O67" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P67" s="2" t="n">
@@ -11213,10 +11217,10 @@
       <c r="M68" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N68" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O68" s="25" t="n">
+      <c r="N68" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O68" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P68" s="2" t="n">
@@ -11294,10 +11298,10 @@
       <c r="M69" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N69" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O69" s="25" t="n">
+      <c r="N69" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O69" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P69" s="2" t="n">
@@ -11375,10 +11379,10 @@
       <c r="M70" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N70" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O70" s="25" t="n">
+      <c r="N70" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O70" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P70" s="2" t="n">
@@ -11456,10 +11460,10 @@
       <c r="M71" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N71" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O71" s="25" t="n">
+      <c r="N71" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O71" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P71" s="2" t="n">
@@ -11537,10 +11541,10 @@
       <c r="M72" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N72" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O72" s="25" t="n">
+      <c r="N72" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O72" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P72" s="2" t="n">
@@ -11620,10 +11624,10 @@
       <c r="M73" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N73" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O73" s="25" t="n">
+      <c r="N73" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O73" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P73" s="2" t="n">
@@ -11705,10 +11709,10 @@
       <c r="M74" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N74" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O74" s="25" t="n">
+      <c r="N74" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O74" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P74" s="2" t="n">
@@ -11752,12 +11756,12 @@
         <v/>
       </c>
     </row>
-    <row r="76" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="26" t="s">
+    <row r="76" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="N76" s="27"/>
-      <c r="O76" s="28"/>
+      <c r="N76" s="28"/>
+      <c r="O76" s="29"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2"/>
@@ -11851,10 +11855,10 @@
       <c r="M78" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N78" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O78" s="25" t="n">
+      <c r="N78" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O78" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P78" s="2" t="n">
@@ -11924,10 +11928,10 @@
       <c r="M79" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N79" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O79" s="25" t="n">
+      <c r="N79" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O79" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P79" s="2" t="n">
@@ -11996,10 +12000,10 @@
       <c r="M80" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N80" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O80" s="25" t="n">
+      <c r="N80" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O80" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P80" s="2" t="n">
@@ -12069,10 +12073,10 @@
       <c r="M81" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N81" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O81" s="25" t="n">
+      <c r="N81" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O81" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P81" s="2" t="n">
@@ -12145,10 +12149,10 @@
       <c r="M82" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N82" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O82" s="25" t="n">
+      <c r="N82" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O82" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P82" s="2" t="n">
@@ -12224,10 +12228,10 @@
       <c r="M83" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N83" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O83" s="25" t="n">
+      <c r="N83" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O83" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P83" s="2" t="n">
@@ -12305,10 +12309,10 @@
       <c r="M84" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N84" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O84" s="25" t="n">
+      <c r="N84" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O84" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P84" s="2" t="n">
@@ -12386,10 +12390,10 @@
       <c r="M85" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N85" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O85" s="25" t="n">
+      <c r="N85" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O85" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P85" s="2" t="n">
@@ -12469,10 +12473,10 @@
       <c r="M86" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N86" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O86" s="25" t="n">
+      <c r="N86" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O86" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P86" s="2" t="n">
@@ -12554,10 +12558,10 @@
       <c r="M87" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="N87" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O87" s="25" t="n">
+      <c r="N87" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O87" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P87" s="2" t="n">
@@ -12639,10 +12643,10 @@
       <c r="M88" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="N88" s="24" t="n">
-        <v>6</v>
-      </c>
-      <c r="O88" s="25" t="n">
+      <c r="N88" s="25" t="n">
+        <v>6</v>
+      </c>
+      <c r="O88" s="26" t="n">
         <v>6</v>
       </c>
       <c r="P88" s="2" t="n">
@@ -12724,10 +12728,10 @@
       <c r="M89" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="N89" s="24" t="n">
-        <v>6</v>
-      </c>
-      <c r="O89" s="25" t="n">
+      <c r="N89" s="25" t="n">
+        <v>6</v>
+      </c>
+      <c r="O89" s="26" t="n">
         <v>6</v>
       </c>
       <c r="P89" s="2" t="n">
@@ -12771,12 +12775,12 @@
         <v/>
       </c>
     </row>
-    <row r="91" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="26" t="s">
+    <row r="91" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="N91" s="27"/>
-      <c r="O91" s="28"/>
+      <c r="N91" s="28"/>
+      <c r="O91" s="29"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2"/>
@@ -12870,10 +12874,10 @@
       <c r="M93" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N93" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O93" s="25" t="n">
+      <c r="N93" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O93" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P93" s="2" t="n">
@@ -12945,10 +12949,10 @@
       <c r="M94" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N94" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O94" s="25" t="n">
+      <c r="N94" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O94" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P94" s="2" t="n">
@@ -13022,10 +13026,10 @@
       <c r="M95" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N95" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O95" s="25" t="n">
+      <c r="N95" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O95" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P95" s="2" t="n">
@@ -13098,10 +13102,10 @@
       <c r="M96" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N96" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O96" s="25" t="n">
+      <c r="N96" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O96" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P96" s="2" t="n">
@@ -13176,10 +13180,10 @@
       <c r="M97" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N97" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O97" s="25" t="n">
+      <c r="N97" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O97" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P97" s="2" t="n">
@@ -13257,10 +13261,10 @@
       <c r="M98" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N98" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O98" s="25" t="n">
+      <c r="N98" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O98" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P98" s="2" t="n">
@@ -13338,10 +13342,10 @@
       <c r="M99" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N99" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O99" s="25" t="n">
+      <c r="N99" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O99" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P99" s="2" t="n">
@@ -13419,10 +13423,10 @@
       <c r="M100" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N100" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O100" s="25" t="n">
+      <c r="N100" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O100" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P100" s="2" t="n">
@@ -13500,10 +13504,10 @@
       <c r="M101" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N101" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O101" s="25" t="n">
+      <c r="N101" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O101" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P101" s="2" t="n">
@@ -13583,10 +13587,10 @@
       <c r="M102" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N102" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O102" s="25" t="n">
+      <c r="N102" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O102" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P102" s="2" t="n">
@@ -13668,10 +13672,10 @@
       <c r="M103" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N103" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O103" s="25" t="n">
+      <c r="N103" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O103" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P103" s="2" t="n">
@@ -13753,10 +13757,10 @@
       <c r="M104" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N104" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O104" s="25" t="n">
+      <c r="N104" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O104" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P104" s="2" t="n">
@@ -13800,12 +13804,12 @@
         <v/>
       </c>
     </row>
-    <row r="106" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="26" t="s">
+    <row r="106" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="N106" s="27"/>
-      <c r="O106" s="28"/>
+      <c r="N106" s="28"/>
+      <c r="O106" s="29"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2"/>
@@ -13899,10 +13903,10 @@
       <c r="M108" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N108" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O108" s="25" t="n">
+      <c r="N108" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O108" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P108" s="2" t="n">
@@ -13973,10 +13977,10 @@
       <c r="M109" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N109" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O109" s="25" t="n">
+      <c r="N109" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O109" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P109" s="2" t="n">
@@ -14050,10 +14054,10 @@
       <c r="M110" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N110" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O110" s="25" t="n">
+      <c r="N110" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O110" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P110" s="2" t="n">
@@ -14129,10 +14133,10 @@
       <c r="M111" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N111" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O111" s="25" t="n">
+      <c r="N111" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O111" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P111" s="2" t="n">
@@ -14210,10 +14214,10 @@
       <c r="M112" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N112" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O112" s="25" t="n">
+      <c r="N112" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O112" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P112" s="2" t="n">
@@ -14291,10 +14295,10 @@
       <c r="M113" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N113" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O113" s="25" t="n">
+      <c r="N113" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O113" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P113" s="2" t="n">
@@ -14372,10 +14376,10 @@
       <c r="M114" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N114" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O114" s="25" t="n">
+      <c r="N114" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O114" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P114" s="2" t="n">
@@ -14453,10 +14457,10 @@
       <c r="M115" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N115" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O115" s="25" t="n">
+      <c r="N115" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O115" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P115" s="2" t="n">
@@ -14534,10 +14538,10 @@
       <c r="M116" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N116" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O116" s="25" t="n">
+      <c r="N116" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O116" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P116" s="2" t="n">
@@ -14617,10 +14621,10 @@
       <c r="M117" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N117" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O117" s="25" t="n">
+      <c r="N117" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O117" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P117" s="2" t="n">
@@ -14702,10 +14706,10 @@
       <c r="M118" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N118" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O118" s="25" t="n">
+      <c r="N118" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O118" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P118" s="2" t="n">
@@ -14789,10 +14793,10 @@
       <c r="M119" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N119" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O119" s="25" t="n">
+      <c r="N119" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O119" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P119" s="2" t="n">
@@ -14838,12 +14842,12 @@
         <v/>
       </c>
     </row>
-    <row r="121" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="26" t="s">
+    <row r="121" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="N121" s="27"/>
-      <c r="O121" s="28"/>
+      <c r="N121" s="28"/>
+      <c r="O121" s="29"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2"/>
@@ -14937,10 +14941,10 @@
       <c r="M123" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N123" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O123" s="25" t="n">
+      <c r="N123" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O123" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P123" s="2" t="n">
@@ -15009,10 +15013,10 @@
       <c r="M124" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N124" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O124" s="25" t="n">
+      <c r="N124" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O124" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P124" s="2" t="n">
@@ -15084,10 +15088,10 @@
       <c r="M125" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N125" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O125" s="25" t="n">
+      <c r="N125" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O125" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P125" s="2" t="n">
@@ -15161,10 +15165,10 @@
       <c r="M126" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N126" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O126" s="25" t="n">
+      <c r="N126" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O126" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P126" s="2" t="n">
@@ -15238,10 +15242,10 @@
       <c r="M127" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N127" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O127" s="25" t="n">
+      <c r="N127" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O127" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P127" s="2" t="n">
@@ -15317,10 +15321,10 @@
       <c r="M128" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N128" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O128" s="25" t="n">
+      <c r="N128" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O128" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P128" s="2" t="n">
@@ -15398,10 +15402,10 @@
       <c r="M129" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N129" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O129" s="25" t="n">
+      <c r="N129" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O129" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P129" s="2" t="n">
@@ -15479,10 +15483,10 @@
       <c r="M130" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N130" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O130" s="25" t="n">
+      <c r="N130" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O130" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P130" s="2" t="n">
@@ -15560,10 +15564,10 @@
       <c r="M131" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N131" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O131" s="25" t="n">
+      <c r="N131" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O131" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P131" s="2" t="n">
@@ -15641,10 +15645,10 @@
       <c r="M132" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N132" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O132" s="25" t="n">
+      <c r="N132" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O132" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P132" s="2" t="n">
@@ -15722,10 +15726,10 @@
       <c r="M133" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N133" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O133" s="25" t="n">
+      <c r="N133" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O133" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P133" s="2" t="n">
@@ -15805,10 +15809,10 @@
       <c r="M134" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N134" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O134" s="25" t="n">
+      <c r="N134" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O134" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P134" s="2" t="n">
@@ -15852,12 +15856,12 @@
         <v/>
       </c>
     </row>
-    <row r="136" s="26" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="26" t="s">
+    <row r="136" s="27" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="N136" s="27"/>
-      <c r="O136" s="28"/>
+      <c r="N136" s="28"/>
+      <c r="O136" s="29"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2"/>
@@ -15951,10 +15955,10 @@
       <c r="M138" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="N138" s="24" t="n">
+      <c r="N138" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="O138" s="25" t="n">
+      <c r="O138" s="26" t="n">
         <v>9</v>
       </c>
       <c r="P138" s="2" t="n">
@@ -16023,10 +16027,10 @@
       <c r="M139" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N139" s="24" t="n">
+      <c r="N139" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="O139" s="25" t="n">
+      <c r="O139" s="26" t="n">
         <v>9</v>
       </c>
       <c r="P139" s="2" t="n">
@@ -16096,10 +16100,10 @@
       <c r="M140" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="N140" s="24" t="n">
+      <c r="N140" s="25" t="n">
         <v>9</v>
       </c>
-      <c r="O140" s="25" t="n">
+      <c r="O140" s="26" t="n">
         <v>9</v>
       </c>
       <c r="P140" s="2" t="n">
@@ -16171,10 +16175,10 @@
       <c r="M141" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N141" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O141" s="25" t="n">
+      <c r="N141" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O141" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P141" s="2" t="n">
@@ -16248,10 +16252,10 @@
       <c r="M142" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N142" s="24" t="n">
-        <v>8</v>
-      </c>
-      <c r="O142" s="25" t="n">
+      <c r="N142" s="25" t="n">
+        <v>8</v>
+      </c>
+      <c r="O142" s="26" t="n">
         <v>8</v>
       </c>
       <c r="P142" s="2" t="n">
@@ -16327,10 +16331,10 @@
       <c r="M143" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N143" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O143" s="25" t="n">
+      <c r="N143" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O143" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P143" s="2" t="n">
@@ -16408,10 +16412,10 @@
       <c r="M144" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N144" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O144" s="25" t="n">
+      <c r="N144" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O144" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P144" s="2" t="n">
@@ -16489,10 +16493,10 @@
       <c r="M145" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N145" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O145" s="25" t="n">
+      <c r="N145" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O145" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P145" s="2" t="n">
@@ -16572,10 +16576,10 @@
       <c r="M146" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N146" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O146" s="25" t="n">
+      <c r="N146" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O146" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P146" s="2" t="n">
@@ -16657,10 +16661,10 @@
       <c r="M147" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N147" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O147" s="25" t="n">
+      <c r="N147" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O147" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P147" s="2" t="n">
@@ -16742,10 +16746,10 @@
       <c r="M148" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N148" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O148" s="25" t="n">
+      <c r="N148" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O148" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P148" s="2" t="n">
@@ -16829,10 +16833,10 @@
       <c r="M149" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="N149" s="24" t="n">
-        <v>7</v>
-      </c>
-      <c r="O149" s="25" t="n">
+      <c r="N149" s="25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O149" s="26" t="n">
         <v>7</v>
       </c>
       <c r="P149" s="2" t="n">
@@ -16896,8 +16900,8 @@
       <c r="K164" s="2"/>
       <c r="L164" s="2"/>
       <c r="M164" s="2"/>
-      <c r="N164" s="24"/>
-      <c r="O164" s="25"/>
+      <c r="N164" s="25"/>
+      <c r="O164" s="26"/>
       <c r="P164" s="2"/>
       <c r="Q164" s="2"/>
       <c r="R164" s="2"/>
@@ -16927,8 +16931,8 @@
       <c r="K165" s="2"/>
       <c r="L165" s="2"/>
       <c r="M165" s="2"/>
-      <c r="N165" s="24"/>
-      <c r="O165" s="25"/>
+      <c r="N165" s="25"/>
+      <c r="O165" s="26"/>
       <c r="P165" s="2"/>
       <c r="Q165" s="2"/>
       <c r="R165" s="2"/>
@@ -16959,8 +16963,8 @@
       <c r="K166" s="2"/>
       <c r="L166" s="2"/>
       <c r="M166" s="2"/>
-      <c r="N166" s="24"/>
-      <c r="O166" s="25"/>
+      <c r="N166" s="25"/>
+      <c r="O166" s="26"/>
       <c r="P166" s="2"/>
       <c r="Q166" s="2"/>
       <c r="R166" s="2"/>
@@ -16991,8 +16995,8 @@
       <c r="K167" s="2"/>
       <c r="L167" s="2"/>
       <c r="M167" s="2"/>
-      <c r="N167" s="24"/>
-      <c r="O167" s="25"/>
+      <c r="N167" s="25"/>
+      <c r="O167" s="26"/>
       <c r="P167" s="2"/>
       <c r="Q167" s="2"/>
       <c r="R167" s="2"/>
@@ -17023,8 +17027,8 @@
       <c r="K168" s="2"/>
       <c r="L168" s="2"/>
       <c r="M168" s="2"/>
-      <c r="N168" s="24"/>
-      <c r="O168" s="25"/>
+      <c r="N168" s="25"/>
+      <c r="O168" s="26"/>
       <c r="P168" s="2"/>
       <c r="Q168" s="2"/>
       <c r="R168" s="2"/>
@@ -17055,8 +17059,8 @@
       <c r="K169" s="2"/>
       <c r="L169" s="2"/>
       <c r="M169" s="2"/>
-      <c r="N169" s="24"/>
-      <c r="O169" s="25"/>
+      <c r="N169" s="25"/>
+      <c r="O169" s="26"/>
       <c r="P169" s="2"/>
       <c r="Q169" s="2"/>
       <c r="R169" s="2"/>
@@ -17087,8 +17091,8 @@
       <c r="K170" s="2"/>
       <c r="L170" s="2"/>
       <c r="M170" s="2"/>
-      <c r="N170" s="24"/>
-      <c r="O170" s="25"/>
+      <c r="N170" s="25"/>
+      <c r="O170" s="26"/>
       <c r="P170" s="2"/>
       <c r="Q170" s="2"/>
       <c r="R170" s="2"/>
@@ -17119,8 +17123,8 @@
       <c r="K171" s="2"/>
       <c r="L171" s="2"/>
       <c r="M171" s="2"/>
-      <c r="N171" s="24"/>
-      <c r="O171" s="25"/>
+      <c r="N171" s="25"/>
+      <c r="O171" s="26"/>
       <c r="P171" s="2"/>
       <c r="Q171" s="2"/>
       <c r="R171" s="2"/>
@@ -17151,8 +17155,8 @@
       <c r="K172" s="2"/>
       <c r="L172" s="2"/>
       <c r="M172" s="2"/>
-      <c r="N172" s="24"/>
-      <c r="O172" s="25"/>
+      <c r="N172" s="25"/>
+      <c r="O172" s="26"/>
       <c r="P172" s="2"/>
       <c r="Q172" s="2"/>
       <c r="R172" s="2"/>
@@ -17183,8 +17187,8 @@
       <c r="K173" s="2"/>
       <c r="L173" s="2"/>
       <c r="M173" s="2"/>
-      <c r="N173" s="24"/>
-      <c r="O173" s="25"/>
+      <c r="N173" s="25"/>
+      <c r="O173" s="26"/>
       <c r="P173" s="2"/>
       <c r="Q173" s="2"/>
       <c r="R173" s="2"/>
@@ -17215,8 +17219,8 @@
       <c r="K174" s="2"/>
       <c r="L174" s="2"/>
       <c r="M174" s="2"/>
-      <c r="N174" s="24"/>
-      <c r="O174" s="25"/>
+      <c r="N174" s="25"/>
+      <c r="O174" s="26"/>
       <c r="P174" s="2"/>
       <c r="Q174" s="2"/>
       <c r="R174" s="2"/>

</xml_diff>